<commit_message>
Version from 2011-08-26. Minor optimization with VLAs. Added comparisons with fast dynamic cast of Gibbs and Stroustrup. Updated TR
</commit_message>
<xml_diff>
--- a/media/papers/TR/DCast-vs-Visitors.xlsx
+++ b/media/papers/TR/DCast-vs-Visitors.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="6"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8400" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8409" uniqueCount="18">
   <si>
     <t>AreaVisSeq</t>
   </si>
@@ -238,6 +238,30 @@
   </si>
   <si>
     <t>AreaMatSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    </t>
+  </si>
+  <si>
+    <t>DT+Mem</t>
+  </si>
+  <si>
+    <t>DT+FDC</t>
+  </si>
+  <si>
+    <t>IF+FDC</t>
+  </si>
+  <si>
+    <t>IF+Mem</t>
+  </si>
+  <si>
+    <t>IF+dc</t>
+  </si>
+  <si>
+    <t>Vis</t>
+  </si>
+  <si>
+    <t>DT+dc</t>
   </si>
 </sst>
 </file>
@@ -281,6 +305,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD2A000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -323,14 +352,17 @@
           <c:idx val="1"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>dynamic_cast</c:v>
+            <c:v>Cascading-If + dynamic_cast</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="15875"/>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$C$1:$C$100</c:f>
+              <c:f>Sheet3!$C$2:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -633,6 +665,331 @@
                 </c:pt>
                 <c:pt idx="99">
                   <c:v>22760</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Decision-Tree + dynamic_cast</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$D$2:$D$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>407</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>697</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>963</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1506</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1493</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1842</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1627</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1923</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2145</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2502</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2193</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2538</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2595</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2927</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2356</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2648</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2722</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>3046</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2978</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3341</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3532</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3742</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>3062</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>3338</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>3407</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3768</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>3539</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>3769</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4105</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>4404</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>3173</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3495</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>3561</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>3850</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>3662</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>3941</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4117</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>4472</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3928</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4297</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4400</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>4671</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4517</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>4835</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5000</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5307</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4010</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>4346</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4361</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>4580</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>4474</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4812</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4808</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5046</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4426</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>4757</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4869</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5154</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5094</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5350</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>5597</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5921</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>3856</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4173</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>4362</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>4653</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>4422</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>4734</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>4894</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>5183</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>4568</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>4866</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>4919</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>5186</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>5057</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>5369</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>5632</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>6394</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>4880</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>5109</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>5187</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>5464</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>5339</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>5593</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>5786</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>6078</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>5506</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>5778</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>5888</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>6153</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>5974</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>6277</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>6503</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>6927</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>4830</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>5126</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>5275</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>5553</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -641,18 +998,16 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
-            <c:v>memoized_cast</c:v>
+            <c:v>Cascading-If + memoized_cast</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln>
+            <a:ln w="19050">
               <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
+                <a:srgbClr val="00B050"/>
               </a:solidFill>
-              <a:prstDash val="solid"/>
+              <a:prstDash val="sysDot"/>
             </a:ln>
           </c:spPr>
           <c:marker>
@@ -660,7 +1015,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$1:$B$100</c:f>
+              <c:f>Sheet3!$B$2:$B$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -971,16 +1326,23 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
-            <c:v>Visitors</c:v>
+            <c:v>Visitor design pattern</c:v>
           </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
           <c:marker>
             <c:symbol val="none"/>
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$A$1:$A$100</c:f>
+              <c:f>Sheet3!$A$2:$A$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1299,20 +1661,46 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="142880128"/>
-        <c:axId val="142910592"/>
+        <c:axId val="42149376"/>
+        <c:axId val="42151296"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="142880128"/>
+        <c:axId val="42149376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Case:</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9868985126859143E-2"/>
+              <c:y val="0.90645815106445027"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142910592"/>
+        <c:crossAx val="42151296"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1320,18 +1708,44 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="142910592"/>
+        <c:axId val="42151296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
         <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.11388888888888889"/>
+              <c:y val="0.39443496646252552"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="142880128"/>
+        <c:crossAx val="42149376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1343,9 +1757,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.14555511811023622"/>
-          <c:y val="6.4430956547098281E-2"/>
-          <c:w val="0.26101443569553806"/>
-          <c:h val="0.25115157480314959"/>
+          <c:y val="8.7579104695246421E-2"/>
+          <c:w val="0.481667760279965"/>
+          <c:h val="0.2538385826771653"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1363,6 +1777,1305 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.11375388724676848"/>
+          <c:y val="5.1400554097404488E-2"/>
+          <c:w val="0.84985570872453686"/>
+          <c:h val="0.8421799358413532"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Cascading-If + memoized_cast</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:srgbClr val="00B050"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>133</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>145</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>157</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>168</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Cascading-If + Fast Dynamic Cast</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:schemeClr val="accent6">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$F$2:$F$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="15"/>
+                <c:pt idx="0">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>147</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Decision-Tree + Fast Dynamic Cast</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="17780">
+              <a:solidFill>
+                <a:srgbClr val="002060"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$E$2:$E$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>38</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>48</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>122</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>125</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>126</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>136</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>113</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>146</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>99</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>119</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Decision-Tree + memoized_cast</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="17780">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$G$2:$G$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>44</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>58</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>53</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>68</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>65</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>82</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>62</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>77</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>72</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>87</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>86</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>93</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>123</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>102</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>134</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>139</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>97</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>112</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>106</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>95</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>84</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>79</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>104</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>119</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>130</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>73</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>105</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>116</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>103</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>132</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>108</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>120</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>140</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>115</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>138</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>127</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>144</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>94</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>114</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>121</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:v>Visitor Design Pattern</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$A$2:$A$101</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="100"/>
+                <c:pt idx="0">
+                  <c:v>39</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>28</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>28</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="42180992"/>
+        <c:axId val="42182528"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="42180992"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Case:</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.962641311180529E-2"/>
+              <c:y val="0.913176097348666"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="42182528"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickLblSkip val="5"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="42182528"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>Cycles</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="42180992"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.45385041388870784"/>
+          <c:y val="0.57593315484961038"/>
+          <c:w val="0.50820406465264012"/>
+          <c:h val="0.3084604850938677"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1000"/>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2362,11 +4075,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="145816192"/>
-        <c:axId val="145822080"/>
+        <c:axId val="56271616"/>
+        <c:axId val="56273152"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="145816192"/>
+        <c:axId val="56271616"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2375,7 +4088,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145822080"/>
+        <c:crossAx val="56273152"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2383,7 +4096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145822080"/>
+        <c:axId val="56273152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2394,7 +4107,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145816192"/>
+        <c:crossAx val="56271616"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2429,16 +4142,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2452,6 +4165,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>9523</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14286</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>314325</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -24220,416 +25963,848 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C100"/>
+  <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q14" sqref="Q14"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S21" sqref="S21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
         <v>39</v>
       </c>
-      <c r="B1">
+      <c r="B2">
         <v>12</v>
       </c>
-      <c r="C1">
+      <c r="C2">
         <v>93</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="D2">
+        <v>115</v>
+      </c>
+      <c r="E2">
+        <v>19</v>
+      </c>
+      <c r="F2">
+        <v>11</v>
+      </c>
+      <c r="G2">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
         <v>32</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>17</v>
       </c>
-      <c r="C2">
+      <c r="C3">
         <v>304</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>28</v>
-      </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <v>407</v>
+      </c>
+      <c r="E3">
+        <v>38</v>
+      </c>
+      <c r="F3">
+        <v>19</v>
+      </c>
+      <c r="G3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>28</v>
       </c>
       <c r="B4">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="C4">
-        <v>742</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>516</v>
+      </c>
+      <c r="D4">
+        <v>697</v>
+      </c>
+      <c r="E4">
+        <v>48</v>
+      </c>
+      <c r="F4">
+        <v>29</v>
+      </c>
+      <c r="G4">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
       <c r="B5">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C5">
-        <v>966</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>742</v>
+      </c>
+      <c r="D5">
+        <v>963</v>
+      </c>
+      <c r="E5">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>38</v>
+      </c>
+      <c r="G5">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="C6">
-        <v>1217</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>966</v>
+      </c>
+      <c r="D6">
+        <v>1147</v>
+      </c>
+      <c r="E6">
+        <v>58</v>
+      </c>
+      <c r="F6">
+        <v>48</v>
+      </c>
+      <c r="G6">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>28</v>
       </c>
       <c r="B7">
-        <v>72</v>
+        <v>61</v>
       </c>
       <c r="C7">
-        <v>1408</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1217</v>
+      </c>
+      <c r="D7">
+        <v>1506</v>
+      </c>
+      <c r="E7">
+        <v>68</v>
+      </c>
+      <c r="F7">
+        <v>58</v>
+      </c>
+      <c r="G7">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
       <c r="B8">
-        <v>84</v>
+        <v>72</v>
       </c>
       <c r="C8">
-        <v>1666</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1408</v>
+      </c>
+      <c r="D8">
+        <v>1493</v>
+      </c>
+      <c r="E8">
+        <v>68</v>
+      </c>
+      <c r="F8">
+        <v>68</v>
+      </c>
+      <c r="G8">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>28</v>
       </c>
       <c r="B9">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C9">
-        <v>1886</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1666</v>
+      </c>
+      <c r="D9">
+        <v>1842</v>
+      </c>
+      <c r="E9">
+        <v>77</v>
+      </c>
+      <c r="F9">
+        <v>77</v>
+      </c>
+      <c r="G9">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
       <c r="B10">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="C10">
-        <v>2088</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+        <v>1886</v>
+      </c>
+      <c r="D10">
+        <v>1627</v>
+      </c>
+      <c r="E10">
+        <v>68</v>
+      </c>
+      <c r="F10">
+        <v>87</v>
+      </c>
+      <c r="G10">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>28</v>
       </c>
       <c r="B11">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="C11">
-        <v>2317</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2088</v>
+      </c>
+      <c r="D11">
+        <v>1923</v>
+      </c>
+      <c r="E11">
+        <v>77</v>
+      </c>
+      <c r="F11">
+        <v>97</v>
+      </c>
+      <c r="G11">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28</v>
       </c>
       <c r="B12">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C12">
-        <v>2520</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2317</v>
+      </c>
+      <c r="D12">
+        <v>2145</v>
+      </c>
+      <c r="E12">
+        <v>77</v>
+      </c>
+      <c r="F12">
+        <v>107</v>
+      </c>
+      <c r="G12">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>28</v>
       </c>
       <c r="B13">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="C13">
-        <v>2821</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2520</v>
+      </c>
+      <c r="D13">
+        <v>2502</v>
+      </c>
+      <c r="E13">
+        <v>87</v>
+      </c>
+      <c r="F13">
+        <v>117</v>
+      </c>
+      <c r="G13">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>28</v>
       </c>
       <c r="B14">
-        <v>157</v>
+        <v>145</v>
       </c>
       <c r="C14">
-        <v>3019</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+        <v>2821</v>
+      </c>
+      <c r="D14">
+        <v>2193</v>
+      </c>
+      <c r="E14">
+        <v>77</v>
+      </c>
+      <c r="F14">
+        <v>126</v>
+      </c>
+      <c r="G14">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>28</v>
       </c>
       <c r="B15">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="C15">
-        <v>3383</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3019</v>
+      </c>
+      <c r="D15">
+        <v>2538</v>
+      </c>
+      <c r="E15">
+        <v>87</v>
+      </c>
+      <c r="F15">
+        <v>136</v>
+      </c>
+      <c r="G15">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>28</v>
       </c>
       <c r="B16">
-        <v>181</v>
+        <v>168</v>
       </c>
       <c r="C16">
-        <v>3577</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3383</v>
+      </c>
+      <c r="D16">
+        <v>2595</v>
+      </c>
+      <c r="E16">
+        <v>87</v>
+      </c>
+      <c r="F16">
+        <v>147</v>
+      </c>
+      <c r="G16">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>28</v>
       </c>
       <c r="B17">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="C17">
-        <v>3820</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3577</v>
+      </c>
+      <c r="D17">
+        <v>2927</v>
+      </c>
+      <c r="E17">
+        <v>97</v>
+      </c>
+      <c r="F17">
+        <v>159</v>
+      </c>
+      <c r="G17">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>28</v>
       </c>
       <c r="B18">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C18">
-        <v>4079</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3820</v>
+      </c>
+      <c r="D18">
+        <v>2356</v>
+      </c>
+      <c r="E18">
+        <v>79</v>
+      </c>
+      <c r="F18">
+        <v>172</v>
+      </c>
+      <c r="G18">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>28</v>
       </c>
       <c r="B19">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C19">
-        <v>4316</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4079</v>
+      </c>
+      <c r="D19">
+        <v>2648</v>
+      </c>
+      <c r="E19">
+        <v>89</v>
+      </c>
+      <c r="F19">
+        <v>176</v>
+      </c>
+      <c r="G19">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>28</v>
       </c>
       <c r="B20">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C20">
-        <v>4540</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4316</v>
+      </c>
+      <c r="D20">
+        <v>2722</v>
+      </c>
+      <c r="E20">
+        <v>89</v>
+      </c>
+      <c r="F20">
+        <v>191</v>
+      </c>
+      <c r="G20">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>28</v>
       </c>
       <c r="B21">
-        <v>240</v>
+        <v>229</v>
       </c>
       <c r="C21">
-        <v>4622</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4540</v>
+      </c>
+      <c r="D21">
+        <v>3046</v>
+      </c>
+      <c r="E21">
+        <v>99</v>
+      </c>
+      <c r="F21">
+        <v>202</v>
+      </c>
+      <c r="G21">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>28</v>
       </c>
       <c r="B22">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C22">
-        <v>4807</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4622</v>
+      </c>
+      <c r="D22">
+        <v>2978</v>
+      </c>
+      <c r="E22">
+        <v>89</v>
+      </c>
+      <c r="F22">
+        <v>211</v>
+      </c>
+      <c r="G22">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>28</v>
       </c>
       <c r="B23">
-        <v>265</v>
+        <v>253</v>
       </c>
       <c r="C23">
-        <v>5054</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4807</v>
+      </c>
+      <c r="D23">
+        <v>3341</v>
+      </c>
+      <c r="E23">
+        <v>99</v>
+      </c>
+      <c r="F23">
+        <v>221</v>
+      </c>
+      <c r="G23">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>28</v>
       </c>
       <c r="B24">
-        <v>277</v>
+        <v>265</v>
       </c>
       <c r="C24">
-        <v>5347</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5054</v>
+      </c>
+      <c r="D24">
+        <v>3532</v>
+      </c>
+      <c r="E24">
+        <v>99</v>
+      </c>
+      <c r="F24">
+        <v>231</v>
+      </c>
+      <c r="G24">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>28</v>
       </c>
       <c r="B25">
-        <v>288</v>
+        <v>277</v>
       </c>
       <c r="C25">
-        <v>5586</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5347</v>
+      </c>
+      <c r="D25">
+        <v>3742</v>
+      </c>
+      <c r="E25">
+        <v>108</v>
+      </c>
+      <c r="F25">
+        <v>241</v>
+      </c>
+      <c r="G25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>28</v>
       </c>
       <c r="B26">
-        <v>302</v>
+        <v>288</v>
       </c>
       <c r="C26">
-        <v>5789</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5586</v>
+      </c>
+      <c r="D26">
+        <v>3062</v>
+      </c>
+      <c r="E26">
+        <v>90</v>
+      </c>
+      <c r="F26">
+        <v>250</v>
+      </c>
+      <c r="G26">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>28</v>
       </c>
       <c r="B27">
-        <v>315</v>
+        <v>302</v>
       </c>
       <c r="C27">
-        <v>6140</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5789</v>
+      </c>
+      <c r="D27">
+        <v>3338</v>
+      </c>
+      <c r="E27">
+        <v>100</v>
+      </c>
+      <c r="F27">
+        <v>260</v>
+      </c>
+      <c r="G27">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28">
-        <v>325</v>
+        <v>315</v>
       </c>
       <c r="C28">
-        <v>6351</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6140</v>
+      </c>
+      <c r="D28">
+        <v>3407</v>
+      </c>
+      <c r="E28">
+        <v>99</v>
+      </c>
+      <c r="F28">
+        <v>270</v>
+      </c>
+      <c r="G28">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
-        <v>337</v>
+        <v>325</v>
       </c>
       <c r="C29">
-        <v>6639</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6351</v>
+      </c>
+      <c r="D29">
+        <v>3768</v>
+      </c>
+      <c r="E29">
+        <v>109</v>
+      </c>
+      <c r="F29">
+        <v>280</v>
+      </c>
+      <c r="G29">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
-        <v>350</v>
+        <v>337</v>
       </c>
       <c r="C30">
-        <v>6896</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6639</v>
+      </c>
+      <c r="D30">
+        <v>3539</v>
+      </c>
+      <c r="E30">
+        <v>99</v>
+      </c>
+      <c r="F30">
+        <v>290</v>
+      </c>
+      <c r="G30">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31">
-        <v>360</v>
+        <v>350</v>
       </c>
       <c r="C31">
-        <v>6959</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6896</v>
+      </c>
+      <c r="D31">
+        <v>3769</v>
+      </c>
+      <c r="E31">
+        <v>109</v>
+      </c>
+      <c r="F31">
+        <v>299</v>
+      </c>
+      <c r="G31">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32">
-        <v>374</v>
+        <v>360</v>
       </c>
       <c r="C32">
-        <v>7183</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+        <v>6959</v>
+      </c>
+      <c r="D32">
+        <v>4105</v>
+      </c>
+      <c r="E32">
+        <v>110</v>
+      </c>
+      <c r="F32">
+        <v>309</v>
+      </c>
+      <c r="G32">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33">
-        <v>388</v>
+        <v>374</v>
       </c>
       <c r="C33">
-        <v>7382</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7183</v>
+      </c>
+      <c r="D33">
+        <v>4404</v>
+      </c>
+      <c r="E33">
+        <v>119</v>
+      </c>
+      <c r="F33">
+        <v>319</v>
+      </c>
+      <c r="G33">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34">
-        <v>398</v>
+        <v>388</v>
       </c>
       <c r="C34">
-        <v>7698</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7382</v>
+      </c>
+      <c r="D34">
+        <v>3173</v>
+      </c>
+      <c r="E34">
+        <v>91</v>
+      </c>
+      <c r="F34">
+        <v>328</v>
+      </c>
+      <c r="G34">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>28</v>
       </c>
       <c r="B35">
-        <v>418</v>
+        <v>398</v>
       </c>
       <c r="C35">
-        <v>7942</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7698</v>
+      </c>
+      <c r="D35">
+        <v>3495</v>
+      </c>
+      <c r="E35">
+        <v>101</v>
+      </c>
+      <c r="F35">
+        <v>338</v>
+      </c>
+      <c r="G35">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
       <c r="B36">
-        <v>436</v>
+        <v>418</v>
       </c>
       <c r="C36">
-        <v>8148</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+        <v>7942</v>
+      </c>
+      <c r="D36">
+        <v>3561</v>
+      </c>
+      <c r="E36">
+        <v>101</v>
+      </c>
+      <c r="F36">
+        <v>348</v>
+      </c>
+      <c r="G36">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
@@ -24637,318 +26812,594 @@
         <v>436</v>
       </c>
       <c r="C37">
-        <v>8304</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8148</v>
+      </c>
+      <c r="D37">
+        <v>3850</v>
+      </c>
+      <c r="E37">
+        <v>111</v>
+      </c>
+      <c r="F37">
+        <v>359</v>
+      </c>
+      <c r="G37">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>28</v>
       </c>
       <c r="B38">
-        <v>449</v>
+        <v>436</v>
       </c>
       <c r="C38">
-        <v>8595</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8304</v>
+      </c>
+      <c r="D38">
+        <v>3662</v>
+      </c>
+      <c r="E38">
+        <v>101</v>
+      </c>
+      <c r="F38">
+        <v>371</v>
+      </c>
+      <c r="G38">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>28</v>
       </c>
       <c r="B39">
-        <v>471</v>
+        <v>449</v>
       </c>
       <c r="C39">
-        <v>8816</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8595</v>
+      </c>
+      <c r="D39">
+        <v>3941</v>
+      </c>
+      <c r="E39">
+        <v>111</v>
+      </c>
+      <c r="F39">
+        <v>378</v>
+      </c>
+      <c r="G39">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>28</v>
       </c>
       <c r="B40">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="C40">
-        <v>8995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8816</v>
+      </c>
+      <c r="D40">
+        <v>4117</v>
+      </c>
+      <c r="E40">
+        <v>111</v>
+      </c>
+      <c r="F40">
+        <v>387</v>
+      </c>
+      <c r="G40">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28</v>
       </c>
       <c r="B41">
-        <v>500</v>
+        <v>487</v>
       </c>
       <c r="C41">
-        <v>9139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+        <v>8995</v>
+      </c>
+      <c r="D41">
+        <v>4472</v>
+      </c>
+      <c r="E41">
+        <v>122</v>
+      </c>
+      <c r="F41">
+        <v>403</v>
+      </c>
+      <c r="G41">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>28</v>
       </c>
       <c r="B42">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C42">
-        <v>9430</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9139</v>
+      </c>
+      <c r="D42">
+        <v>3928</v>
+      </c>
+      <c r="E42">
+        <v>102</v>
+      </c>
+      <c r="G42">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>28</v>
       </c>
       <c r="B43">
-        <v>514</v>
+        <v>503</v>
       </c>
       <c r="C43">
-        <v>9637</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9430</v>
+      </c>
+      <c r="D43">
+        <v>4297</v>
+      </c>
+      <c r="E43">
+        <v>112</v>
+      </c>
+      <c r="G43">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>28</v>
       </c>
       <c r="B44">
-        <v>537</v>
+        <v>514</v>
       </c>
       <c r="C44">
-        <v>10005</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>9637</v>
+      </c>
+      <c r="D44">
+        <v>4400</v>
+      </c>
+      <c r="E44">
+        <v>112</v>
+      </c>
+      <c r="G44">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>28</v>
       </c>
       <c r="B45">
-        <v>533</v>
+        <v>537</v>
       </c>
       <c r="C45">
-        <v>10247</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10005</v>
+      </c>
+      <c r="D45">
+        <v>4671</v>
+      </c>
+      <c r="E45">
+        <v>125</v>
+      </c>
+      <c r="G45">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>28</v>
       </c>
       <c r="B46">
-        <v>546</v>
+        <v>533</v>
       </c>
       <c r="C46">
-        <v>10483</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10247</v>
+      </c>
+      <c r="D46">
+        <v>4517</v>
+      </c>
+      <c r="E46">
+        <v>113</v>
+      </c>
+      <c r="G46">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>28</v>
       </c>
       <c r="B47">
-        <v>559</v>
+        <v>546</v>
       </c>
       <c r="C47">
-        <v>10753</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10483</v>
+      </c>
+      <c r="D47">
+        <v>4835</v>
+      </c>
+      <c r="E47">
+        <v>122</v>
+      </c>
+      <c r="G47">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>28</v>
       </c>
       <c r="B48">
-        <v>589</v>
+        <v>559</v>
       </c>
       <c r="C48">
-        <v>10966</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10753</v>
+      </c>
+      <c r="D48">
+        <v>5000</v>
+      </c>
+      <c r="E48">
+        <v>125</v>
+      </c>
+      <c r="G48">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>28</v>
       </c>
       <c r="B49">
-        <v>583</v>
+        <v>589</v>
       </c>
       <c r="C49">
-        <v>11036</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+        <v>10966</v>
+      </c>
+      <c r="D49">
+        <v>5307</v>
+      </c>
+      <c r="E49">
+        <v>139</v>
+      </c>
+      <c r="G49">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>28</v>
       </c>
       <c r="B50">
-        <v>594</v>
+        <v>583</v>
       </c>
       <c r="C50">
-        <v>11422</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11036</v>
+      </c>
+      <c r="D50">
+        <v>4010</v>
+      </c>
+      <c r="E50">
+        <v>103</v>
+      </c>
+      <c r="G50">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>28</v>
       </c>
       <c r="B51">
-        <v>623</v>
+        <v>594</v>
       </c>
       <c r="C51">
-        <v>11358</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11422</v>
+      </c>
+      <c r="D51">
+        <v>4346</v>
+      </c>
+      <c r="E51">
+        <v>114</v>
+      </c>
+      <c r="G51">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>28</v>
       </c>
       <c r="B52">
-        <v>618</v>
+        <v>623</v>
       </c>
       <c r="C52">
-        <v>11603</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11358</v>
+      </c>
+      <c r="D52">
+        <v>4361</v>
+      </c>
+      <c r="E52">
+        <v>93</v>
+      </c>
+      <c r="G52">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>28</v>
       </c>
       <c r="B53">
-        <v>646</v>
+        <v>618</v>
       </c>
       <c r="C53">
-        <v>11923</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11603</v>
+      </c>
+      <c r="D53">
+        <v>4580</v>
+      </c>
+      <c r="E53">
+        <v>103</v>
+      </c>
+      <c r="G53">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>28</v>
       </c>
       <c r="B54">
-        <v>644</v>
+        <v>646</v>
       </c>
       <c r="C54">
-        <v>12103</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+        <v>11923</v>
+      </c>
+      <c r="D54">
+        <v>4474</v>
+      </c>
+      <c r="E54">
+        <v>93</v>
+      </c>
+      <c r="G54">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>28</v>
       </c>
       <c r="B55">
-        <v>657</v>
+        <v>644</v>
       </c>
       <c r="C55">
-        <v>12315</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12103</v>
+      </c>
+      <c r="D55">
+        <v>4812</v>
+      </c>
+      <c r="E55">
+        <v>103</v>
+      </c>
+      <c r="G55">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>28</v>
       </c>
       <c r="B56">
-        <v>671</v>
+        <v>657</v>
       </c>
       <c r="C56">
-        <v>12773</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12315</v>
+      </c>
+      <c r="D56">
+        <v>4808</v>
+      </c>
+      <c r="E56">
+        <v>103</v>
+      </c>
+      <c r="G56">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>28</v>
       </c>
       <c r="B57">
-        <v>690</v>
+        <v>671</v>
       </c>
       <c r="C57">
-        <v>13024</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12773</v>
+      </c>
+      <c r="D57">
+        <v>5046</v>
+      </c>
+      <c r="E57">
+        <v>113</v>
+      </c>
+      <c r="G57">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>28</v>
       </c>
       <c r="B58">
-        <v>691</v>
+        <v>690</v>
       </c>
       <c r="C58">
-        <v>12945</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13024</v>
+      </c>
+      <c r="D58">
+        <v>4426</v>
+      </c>
+      <c r="E58">
+        <v>94</v>
+      </c>
+      <c r="G58">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>28</v>
       </c>
       <c r="B59">
-        <v>726</v>
+        <v>691</v>
       </c>
       <c r="C59">
-        <v>13485</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+        <v>12945</v>
+      </c>
+      <c r="D59">
+        <v>4757</v>
+      </c>
+      <c r="E59">
+        <v>104</v>
+      </c>
+      <c r="G59">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>28</v>
       </c>
       <c r="B60">
-        <v>725</v>
+        <v>726</v>
       </c>
       <c r="C60">
-        <v>13891</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13485</v>
+      </c>
+      <c r="D60">
+        <v>4869</v>
+      </c>
+      <c r="E60">
+        <v>104</v>
+      </c>
+      <c r="G60">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>28</v>
       </c>
       <c r="B61">
-        <v>742</v>
+        <v>725</v>
       </c>
       <c r="C61">
-        <v>14363</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13891</v>
+      </c>
+      <c r="D61">
+        <v>5154</v>
+      </c>
+      <c r="E61">
+        <v>114</v>
+      </c>
+      <c r="G61">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>28</v>
       </c>
       <c r="B62">
-        <v>738</v>
+        <v>742</v>
       </c>
       <c r="C62">
-        <v>13968</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14363</v>
+      </c>
+      <c r="D62">
+        <v>5094</v>
+      </c>
+      <c r="E62">
+        <v>104</v>
+      </c>
+      <c r="G62">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>28</v>
       </c>
       <c r="B63">
-        <v>764</v>
+        <v>738</v>
       </c>
       <c r="C63">
-        <v>14345</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+        <v>13968</v>
+      </c>
+      <c r="D63">
+        <v>5350</v>
+      </c>
+      <c r="E63">
+        <v>116</v>
+      </c>
+      <c r="G63">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
       <c r="B64">
-        <v>761</v>
+        <v>764</v>
       </c>
       <c r="C64">
-        <v>15087</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14345</v>
+      </c>
+      <c r="D64">
+        <v>5597</v>
+      </c>
+      <c r="E64">
+        <v>115</v>
+      </c>
+      <c r="G64">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>28</v>
       </c>
       <c r="B65">
-        <v>785</v>
+        <v>761</v>
       </c>
       <c r="C65">
-        <v>14872</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15087</v>
+      </c>
+      <c r="D65">
+        <v>5921</v>
+      </c>
+      <c r="E65">
+        <v>126</v>
+      </c>
+      <c r="G65">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>28</v>
       </c>
@@ -24956,386 +27407,730 @@
         <v>785</v>
       </c>
       <c r="C66">
-        <v>15057</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+        <v>14872</v>
+      </c>
+      <c r="D66">
+        <v>3856</v>
+      </c>
+      <c r="E66">
+        <v>85</v>
+      </c>
+      <c r="G66">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>28</v>
       </c>
       <c r="B67">
-        <v>813</v>
+        <v>785</v>
       </c>
       <c r="C67">
-        <v>15287</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15057</v>
+      </c>
+      <c r="D67">
+        <v>4173</v>
+      </c>
+      <c r="E67">
+        <v>95</v>
+      </c>
+      <c r="G67">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>28</v>
       </c>
       <c r="B68">
-        <v>819</v>
+        <v>813</v>
       </c>
       <c r="C68">
-        <v>15505</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15287</v>
+      </c>
+      <c r="D68">
+        <v>4362</v>
+      </c>
+      <c r="E68">
+        <v>95</v>
+      </c>
+      <c r="G68">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>28</v>
       </c>
       <c r="B69">
-        <v>845</v>
+        <v>819</v>
       </c>
       <c r="C69">
-        <v>15618</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15505</v>
+      </c>
+      <c r="D69">
+        <v>4653</v>
+      </c>
+      <c r="E69">
+        <v>105</v>
+      </c>
+      <c r="G69">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>28</v>
       </c>
       <c r="B70">
-        <v>834</v>
+        <v>845</v>
       </c>
       <c r="C70">
-        <v>16027</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+        <v>15618</v>
+      </c>
+      <c r="D70">
+        <v>4422</v>
+      </c>
+      <c r="E70">
+        <v>95</v>
+      </c>
+      <c r="G70">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>28</v>
       </c>
       <c r="B71">
-        <v>868</v>
+        <v>834</v>
       </c>
       <c r="C71">
-        <v>16087</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16027</v>
+      </c>
+      <c r="D71">
+        <v>4734</v>
+      </c>
+      <c r="E71">
+        <v>105</v>
+      </c>
+      <c r="G71">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28</v>
       </c>
       <c r="B72">
-        <v>859</v>
+        <v>868</v>
       </c>
       <c r="C72">
-        <v>16261</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16087</v>
+      </c>
+      <c r="D72">
+        <v>4894</v>
+      </c>
+      <c r="E72">
+        <v>105</v>
+      </c>
+      <c r="G72">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>28</v>
       </c>
       <c r="B73">
-        <v>971</v>
+        <v>859</v>
       </c>
       <c r="C73">
-        <v>16452</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16261</v>
+      </c>
+      <c r="D73">
+        <v>5183</v>
+      </c>
+      <c r="E73">
+        <v>115</v>
+      </c>
+      <c r="G73">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
       <c r="B74">
-        <v>943</v>
+        <v>971</v>
       </c>
       <c r="C74">
-        <v>16658</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16452</v>
+      </c>
+      <c r="D74">
+        <v>4568</v>
+      </c>
+      <c r="E74">
+        <v>96</v>
+      </c>
+      <c r="G74">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>28</v>
       </c>
       <c r="B75">
-        <v>1074</v>
+        <v>943</v>
       </c>
       <c r="C75">
-        <v>17113</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+        <v>16658</v>
+      </c>
+      <c r="D75">
+        <v>4866</v>
+      </c>
+      <c r="E75">
+        <v>106</v>
+      </c>
+      <c r="G75">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>28</v>
       </c>
       <c r="B76">
-        <v>1062</v>
+        <v>1074</v>
       </c>
       <c r="C76">
-        <v>17208</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17113</v>
+      </c>
+      <c r="D76">
+        <v>4919</v>
+      </c>
+      <c r="E76">
+        <v>106</v>
+      </c>
+      <c r="G76">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>28</v>
       </c>
       <c r="B77">
-        <v>1096</v>
+        <v>1062</v>
       </c>
       <c r="C77">
-        <v>17319</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17208</v>
+      </c>
+      <c r="D77">
+        <v>5186</v>
+      </c>
+      <c r="E77">
+        <v>121</v>
+      </c>
+      <c r="G77">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>28</v>
       </c>
       <c r="B78">
-        <v>1053</v>
+        <v>1096</v>
       </c>
       <c r="C78">
-        <v>17733</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17319</v>
+      </c>
+      <c r="D78">
+        <v>5057</v>
+      </c>
+      <c r="E78">
+        <v>110</v>
+      </c>
+      <c r="G78">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>28</v>
       </c>
       <c r="B79">
-        <v>1061</v>
+        <v>1053</v>
       </c>
       <c r="C79">
-        <v>18072</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+        <v>17733</v>
+      </c>
+      <c r="D79">
+        <v>5369</v>
+      </c>
+      <c r="E79">
+        <v>120</v>
+      </c>
+      <c r="G79">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>28</v>
       </c>
       <c r="B80">
-        <v>1101</v>
+        <v>1061</v>
       </c>
       <c r="C80">
-        <v>18269</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18072</v>
+      </c>
+      <c r="D80">
+        <v>5632</v>
+      </c>
+      <c r="E80">
+        <v>121</v>
+      </c>
+      <c r="G80">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>28</v>
       </c>
       <c r="B81">
-        <v>1106</v>
+        <v>1101</v>
       </c>
       <c r="C81">
-        <v>18417</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18269</v>
+      </c>
+      <c r="D81">
+        <v>6394</v>
+      </c>
+      <c r="E81">
+        <v>136</v>
+      </c>
+      <c r="G81">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>28</v>
       </c>
       <c r="B82">
-        <v>1129</v>
+        <v>1106</v>
       </c>
       <c r="C82">
-        <v>18473</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18417</v>
+      </c>
+      <c r="D82">
+        <v>4880</v>
+      </c>
+      <c r="E82">
+        <v>100</v>
+      </c>
+      <c r="G82">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>28</v>
       </c>
       <c r="B83">
-        <v>1139</v>
+        <v>1129</v>
       </c>
       <c r="C83">
-        <v>18575</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18473</v>
+      </c>
+      <c r="D83">
+        <v>5109</v>
+      </c>
+      <c r="E83">
+        <v>110</v>
+      </c>
+      <c r="G83">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>28</v>
       </c>
       <c r="B84">
-        <v>1112</v>
+        <v>1139</v>
       </c>
       <c r="C84">
-        <v>19232</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+        <v>18575</v>
+      </c>
+      <c r="D84">
+        <v>5187</v>
+      </c>
+      <c r="E84">
+        <v>110</v>
+      </c>
+      <c r="G84">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>28</v>
       </c>
       <c r="B85">
-        <v>1225</v>
+        <v>1112</v>
       </c>
       <c r="C85">
-        <v>19420</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19232</v>
+      </c>
+      <c r="D85">
+        <v>5464</v>
+      </c>
+      <c r="E85">
+        <v>121</v>
+      </c>
+      <c r="G85">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>28</v>
       </c>
       <c r="B86">
-        <v>1193</v>
+        <v>1225</v>
       </c>
       <c r="C86">
-        <v>19689</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19420</v>
+      </c>
+      <c r="D86">
+        <v>5339</v>
+      </c>
+      <c r="E86">
+        <v>110</v>
+      </c>
+      <c r="G86">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>28</v>
       </c>
       <c r="B87">
-        <v>1197</v>
+        <v>1193</v>
       </c>
       <c r="C87">
-        <v>19883</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19689</v>
+      </c>
+      <c r="D87">
+        <v>5593</v>
+      </c>
+      <c r="E87">
+        <v>121</v>
+      </c>
+      <c r="G87">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>28</v>
       </c>
       <c r="B88">
-        <v>1243</v>
+        <v>1197</v>
       </c>
       <c r="C88">
-        <v>20094</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+        <v>19883</v>
+      </c>
+      <c r="D88">
+        <v>5786</v>
+      </c>
+      <c r="E88">
+        <v>121</v>
+      </c>
+      <c r="G88">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
       </c>
       <c r="B89">
-        <v>1370</v>
+        <v>1243</v>
       </c>
       <c r="C89">
-        <v>20261</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20094</v>
+      </c>
+      <c r="D89">
+        <v>6078</v>
+      </c>
+      <c r="E89">
+        <v>131</v>
+      </c>
+      <c r="G89">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>28</v>
       </c>
       <c r="B90">
-        <v>1368</v>
+        <v>1370</v>
       </c>
       <c r="C90">
-        <v>20531</v>
-      </c>
-    </row>
-    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20261</v>
+      </c>
+      <c r="D90">
+        <v>5506</v>
+      </c>
+      <c r="E90">
+        <v>113</v>
+      </c>
+      <c r="G90">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>28</v>
       </c>
       <c r="B91">
-        <v>1392</v>
+        <v>1368</v>
       </c>
       <c r="C91">
-        <v>20622</v>
-      </c>
-    </row>
-    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20531</v>
+      </c>
+      <c r="D91">
+        <v>5778</v>
+      </c>
+      <c r="E91">
+        <v>120</v>
+      </c>
+      <c r="G91">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>28</v>
       </c>
       <c r="B92">
-        <v>1411</v>
+        <v>1392</v>
       </c>
       <c r="C92">
-        <v>20838</v>
-      </c>
-    </row>
-    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20622</v>
+      </c>
+      <c r="D92">
+        <v>5888</v>
+      </c>
+      <c r="E92">
+        <v>121</v>
+      </c>
+      <c r="G92">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>28</v>
       </c>
       <c r="B93">
-        <v>1451</v>
+        <v>1411</v>
       </c>
       <c r="C93">
-        <v>20890</v>
-      </c>
-    </row>
-    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20838</v>
+      </c>
+      <c r="D93">
+        <v>6153</v>
+      </c>
+      <c r="E93">
+        <v>130</v>
+      </c>
+      <c r="G93">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>28</v>
       </c>
       <c r="B94">
-        <v>1389</v>
+        <v>1451</v>
       </c>
       <c r="C94">
-        <v>21338</v>
-      </c>
-    </row>
-    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+        <v>20890</v>
+      </c>
+      <c r="D94">
+        <v>5974</v>
+      </c>
+      <c r="E94">
+        <v>120</v>
+      </c>
+      <c r="G94">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>28</v>
       </c>
       <c r="B95">
-        <v>1436</v>
+        <v>1389</v>
       </c>
       <c r="C95">
-        <v>21711</v>
-      </c>
-    </row>
-    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21338</v>
+      </c>
+      <c r="D95">
+        <v>6277</v>
+      </c>
+      <c r="E95">
+        <v>130</v>
+      </c>
+      <c r="G95">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>28</v>
       </c>
       <c r="B96">
-        <v>1449</v>
+        <v>1436</v>
       </c>
       <c r="C96">
-        <v>21958</v>
-      </c>
-    </row>
-    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21711</v>
+      </c>
+      <c r="D96">
+        <v>6503</v>
+      </c>
+      <c r="E96">
+        <v>132</v>
+      </c>
+      <c r="G96">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>28</v>
       </c>
       <c r="B97">
-        <v>1498</v>
+        <v>1449</v>
       </c>
       <c r="C97">
-        <v>22072</v>
-      </c>
-    </row>
-    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+        <v>21958</v>
+      </c>
+      <c r="D97">
+        <v>6927</v>
+      </c>
+      <c r="E97">
+        <v>146</v>
+      </c>
+      <c r="G97">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>28</v>
       </c>
       <c r="B98">
-        <v>1500</v>
+        <v>1498</v>
       </c>
       <c r="C98">
-        <v>22400</v>
-      </c>
-    </row>
-    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22072</v>
+      </c>
+      <c r="D98">
+        <v>4830</v>
+      </c>
+      <c r="E98">
+        <v>99</v>
+      </c>
+      <c r="G98">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>28</v>
       </c>
       <c r="B99">
-        <v>1494</v>
+        <v>1500</v>
       </c>
       <c r="C99">
-        <v>22555</v>
-      </c>
-    </row>
-    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+        <v>22400</v>
+      </c>
+      <c r="D99">
+        <v>5126</v>
+      </c>
+      <c r="E99">
+        <v>109</v>
+      </c>
+      <c r="G99">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>28</v>
       </c>
       <c r="B100">
+        <v>1494</v>
+      </c>
+      <c r="C100">
+        <v>22555</v>
+      </c>
+      <c r="D100">
+        <v>5275</v>
+      </c>
+      <c r="E100">
+        <v>110</v>
+      </c>
+      <c r="G100">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A101">
+        <v>28</v>
+      </c>
+      <c r="B101">
         <v>1464</v>
       </c>
-      <c r="C100">
+      <c r="C101">
         <v>22760</v>
+      </c>
+      <c r="D101">
+        <v>5553</v>
+      </c>
+      <c r="E101">
+        <v>119</v>
+      </c>
+      <c r="G101">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E102" t="s">
+        <v>10</v>
+      </c>
+      <c r="G102" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -39619,7 +42414,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T1" sqref="T1:T1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Version from 2011-08-28. Updated TR
</commit_message>
<xml_diff>
--- a/media/papers/TR/DCast-vs-Visitors.xlsx
+++ b/media/papers/TR/DCast-vs-Visitors.xlsx
@@ -25965,8 +25965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Version from 2011-09-07. Improvements to memoized_cast to allocate less tables. Added files to experiments with DLLs. Updated TR
</commit_message>
<xml_diff>
--- a/media/papers/TR/DCast-vs-Visitors.xlsx
+++ b/media/papers/TR/DCast-vs-Visitors.xlsx
@@ -208,7 +208,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8410" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8411" uniqueCount="20">
   <si>
     <t>AreaVisSeq</t>
   </si>
@@ -265,6 +265,9 @@
   </si>
   <si>
     <t>Our</t>
+  </si>
+  <si>
+    <t>Exception</t>
   </si>
 </sst>
 </file>
@@ -352,8 +355,207 @@
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
+          <c:idx val="4"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Polymorphic Exception</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="15875">
+              <a:solidFill>
+                <a:srgbClr val="00B0F0"/>
+              </a:solidFill>
+              <a:prstDash val="lgDashDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$2:$B$58</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="57"/>
+                <c:pt idx="0">
+                  <c:v>7115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7563</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>7829</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7998</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8332</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8585</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8924</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9228</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9438</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9770</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10034</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10284</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>10636</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>10930</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11301</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>11645</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>11880</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>12127</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>12471</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>12689</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>12858</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>13180</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>13497</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>13885</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>14152</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>14399</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>14585</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>14873</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>15192</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>15611</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>15626</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>15970</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>16303</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>16685</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>17062</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>17153</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>17582</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>17856</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>18087</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>18394</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>18523</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>18855</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>19177</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>19577</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>19831</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>20050</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>20349</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20780</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>21038</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>21362</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>21371</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>21659</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>21980</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>22320</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>22608</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>22964</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>23293</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
           <c:idx val="1"/>
-          <c:order val="0"/>
+          <c:order val="1"/>
           <c:tx>
             <c:v>Cascading-If + dynamic_cast</c:v>
           </c:tx>
@@ -365,7 +567,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$C$2:$C$101</c:f>
+              <c:f>Sheet3!$D$2:$D$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -676,7 +878,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
-          <c:order val="1"/>
+          <c:order val="2"/>
           <c:tx>
             <c:v>Decision-Tree + dynamic_cast</c:v>
           </c:tx>
@@ -690,7 +892,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$D$2:$D$101</c:f>
+              <c:f>Sheet3!$E$2:$E$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1001,7 +1203,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
-          <c:order val="2"/>
+          <c:order val="3"/>
           <c:tx>
             <c:v>Cascading-If + memoized_cast</c:v>
           </c:tx>
@@ -1018,7 +1220,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$101</c:f>
+              <c:f>Sheet3!$C$2:$C$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -1329,7 +1531,7 @@
         </c:ser>
         <c:ser>
           <c:idx val="0"/>
-          <c:order val="3"/>
+          <c:order val="4"/>
           <c:tx>
             <c:v>Visitor design pattern</c:v>
           </c:tx>
@@ -1664,11 +1866,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174045440"/>
-        <c:axId val="174059904"/>
+        <c:axId val="145209600"/>
+        <c:axId val="143720832"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174045440"/>
+        <c:axId val="145209600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1905,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174059904"/>
+        <c:crossAx val="143720832"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1711,7 +1913,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174059904"/>
+        <c:axId val="143720832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1748,7 +1950,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174045440"/>
+        <c:crossAx val="145209600"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1759,10 +1961,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.14555511811023622"/>
+          <c:x val="0.11222178477690288"/>
           <c:y val="8.7579104695246421E-2"/>
-          <c:w val="0.481667760279965"/>
-          <c:h val="0.2538385826771653"/>
+          <c:w val="0.46795888013998249"/>
+          <c:h val="0.29087561971420234"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="0"/>
@@ -1828,7 +2030,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$B$2:$B$16</c:f>
+              <c:f>Sheet3!$C$2:$C$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1902,7 +2104,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$F$2:$F$16</c:f>
+              <c:f>Sheet3!$G$2:$G$16</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
@@ -1975,7 +2177,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$E$2:$E$101</c:f>
+              <c:f>Sheet3!$F$2:$F$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2303,7 +2505,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$G$2:$G$101</c:f>
+              <c:f>Sheet3!$H$2:$H$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -2957,7 +3159,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Sheet3!$H$2:$H$101</c:f>
+              <c:f>Sheet3!$I$2:$I$101</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="100"/>
@@ -3276,11 +3478,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="174685568"/>
-        <c:axId val="174687744"/>
+        <c:axId val="143761792"/>
+        <c:axId val="143763712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="174685568"/>
+        <c:axId val="143761792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3325,7 +3527,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="174687744"/>
+        <c:crossAx val="143763712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3334,7 +3536,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="174687744"/>
+        <c:axId val="143763712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3364,7 +3566,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="174685568"/>
+        <c:crossAx val="143761792"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4405,11 +4607,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="175018752"/>
-        <c:axId val="175020288"/>
+        <c:axId val="148678144"/>
+        <c:axId val="148679680"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="175018752"/>
+        <c:axId val="148678144"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4418,7 +4620,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175020288"/>
+        <c:crossAx val="148679680"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -4426,7 +4628,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="175020288"/>
+        <c:axId val="148679680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4437,7 +4639,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="175018752"/>
+        <c:crossAx val="148678144"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4472,13 +4674,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>16</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>90487</xdr:rowOff>
@@ -4502,13 +4704,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>9523</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>14286</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
+      <xdr:col>24</xdr:col>
       <xdr:colOff>314325</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>95249</xdr:rowOff>
@@ -26293,2470 +26495,2774 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:I102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P9" zoomScale="300" zoomScaleNormal="300" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>15</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>17</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>39</v>
       </c>
       <c r="B2">
+        <v>7115</v>
+      </c>
+      <c r="C2">
         <v>12</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>93</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>115</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>19</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>11</v>
       </c>
-      <c r="G2">
+      <c r="H2">
         <v>19</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>32</v>
       </c>
       <c r="B3">
+        <v>7563</v>
+      </c>
+      <c r="C3">
         <v>17</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>304</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>407</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>38</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>19</v>
       </c>
-      <c r="G3">
+      <c r="H3">
         <v>31</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>28</v>
       </c>
       <c r="B4">
+        <v>7829</v>
+      </c>
+      <c r="C4">
         <v>30</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>516</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>697</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>48</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>29</v>
       </c>
-      <c r="G4">
+      <c r="H4">
         <v>44</v>
       </c>
-      <c r="H4">
+      <c r="I4">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>28</v>
       </c>
       <c r="B5">
+        <v>7998</v>
+      </c>
+      <c r="C5">
         <v>39</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>742</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>963</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>58</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>38</v>
       </c>
-      <c r="G5">
+      <c r="H5">
         <v>58</v>
       </c>
-      <c r="H5">
+      <c r="I5">
         <v>17</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>28</v>
       </c>
       <c r="B6">
+        <v>8332</v>
+      </c>
+      <c r="C6">
         <v>50</v>
       </c>
-      <c r="C6">
+      <c r="D6">
         <v>966</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>1147</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>58</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>48</v>
       </c>
-      <c r="G6">
+      <c r="H6">
         <v>53</v>
       </c>
-      <c r="H6">
+      <c r="I6">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>28</v>
       </c>
       <c r="B7">
+        <v>8585</v>
+      </c>
+      <c r="C7">
         <v>61</v>
       </c>
-      <c r="C7">
+      <c r="D7">
         <v>1217</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1506</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>68</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>58</v>
       </c>
-      <c r="G7">
+      <c r="H7">
         <v>68</v>
       </c>
-      <c r="H7">
+      <c r="I7">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>28</v>
       </c>
       <c r="B8">
+        <v>8924</v>
+      </c>
+      <c r="C8">
         <v>72</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>1408</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>1493</v>
-      </c>
-      <c r="E8">
-        <v>68</v>
       </c>
       <c r="F8">
         <v>68</v>
       </c>
       <c r="G8">
+        <v>68</v>
+      </c>
+      <c r="H8">
         <v>65</v>
       </c>
-      <c r="H8">
+      <c r="I8">
         <v>17</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>28</v>
       </c>
       <c r="B9">
+        <v>9228</v>
+      </c>
+      <c r="C9">
         <v>84</v>
       </c>
-      <c r="C9">
+      <c r="D9">
         <v>1666</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1842</v>
-      </c>
-      <c r="E9">
-        <v>77</v>
       </c>
       <c r="F9">
         <v>77</v>
       </c>
       <c r="G9">
+        <v>77</v>
+      </c>
+      <c r="H9">
         <v>82</v>
       </c>
-      <c r="H9">
+      <c r="I9">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>28</v>
       </c>
       <c r="B10">
+        <v>9438</v>
+      </c>
+      <c r="C10">
         <v>97</v>
       </c>
-      <c r="C10">
+      <c r="D10">
         <v>1886</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1627</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>68</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>87</v>
       </c>
-      <c r="G10">
+      <c r="H10">
         <v>62</v>
       </c>
-      <c r="H10">
+      <c r="I10">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>28</v>
       </c>
       <c r="B11">
+        <v>9770</v>
+      </c>
+      <c r="C11">
         <v>110</v>
       </c>
-      <c r="C11">
+      <c r="D11">
         <v>2088</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1923</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>77</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>97</v>
       </c>
-      <c r="G11">
+      <c r="H11">
         <v>79</v>
       </c>
-      <c r="H11">
+      <c r="I11">
         <v>17</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>28</v>
       </c>
       <c r="B12">
+        <v>10034</v>
+      </c>
+      <c r="C12">
         <v>121</v>
       </c>
-      <c r="C12">
+      <c r="D12">
         <v>2317</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>2145</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>77</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>107</v>
       </c>
-      <c r="G12">
+      <c r="H12">
         <v>77</v>
       </c>
-      <c r="H12">
+      <c r="I12">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>28</v>
       </c>
       <c r="B13">
+        <v>10284</v>
+      </c>
+      <c r="C13">
         <v>133</v>
       </c>
-      <c r="C13">
+      <c r="D13">
         <v>2520</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2502</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>87</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>117</v>
       </c>
-      <c r="G13">
+      <c r="H13">
         <v>91</v>
       </c>
-      <c r="H13">
+      <c r="I13">
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>28</v>
       </c>
       <c r="B14">
+        <v>10636</v>
+      </c>
+      <c r="C14">
         <v>145</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>2821</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2193</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>77</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>126</v>
       </c>
-      <c r="G14">
+      <c r="H14">
         <v>72</v>
       </c>
-      <c r="H14">
+      <c r="I14">
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>28</v>
       </c>
       <c r="B15">
+        <v>10930</v>
+      </c>
+      <c r="C15">
         <v>157</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>3019</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>2538</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>87</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>136</v>
       </c>
-      <c r="G15">
+      <c r="H15">
         <v>92</v>
       </c>
-      <c r="H15">
+      <c r="I15">
         <v>17</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>28</v>
       </c>
       <c r="B16">
+        <v>11301</v>
+      </c>
+      <c r="C16">
         <v>168</v>
       </c>
-      <c r="C16">
+      <c r="D16">
         <v>3383</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>2595</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>87</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>147</v>
       </c>
-      <c r="G16">
+      <c r="H16">
         <v>94</v>
       </c>
-      <c r="H16">
+      <c r="I16">
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>28</v>
       </c>
       <c r="B17">
+        <v>11645</v>
+      </c>
+      <c r="C17">
         <v>181</v>
       </c>
-      <c r="C17">
+      <c r="D17">
         <v>3577</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>2927</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>97</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>159</v>
       </c>
-      <c r="G17">
+      <c r="H17">
         <v>106</v>
       </c>
-      <c r="H17">
+      <c r="I17">
         <v>17</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>28</v>
       </c>
       <c r="B18">
+        <v>11880</v>
+      </c>
+      <c r="C18">
         <v>194</v>
       </c>
-      <c r="C18">
+      <c r="D18">
         <v>3820</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>2356</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>79</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>172</v>
       </c>
-      <c r="G18">
+      <c r="H18">
         <v>73</v>
       </c>
-      <c r="H18">
+      <c r="I18">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>28</v>
       </c>
       <c r="B19">
+        <v>12127</v>
+      </c>
+      <c r="C19">
         <v>205</v>
       </c>
-      <c r="C19">
+      <c r="D19">
         <v>4079</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>2648</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>89</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>176</v>
       </c>
-      <c r="G19">
+      <c r="H19">
         <v>93</v>
       </c>
-      <c r="H19">
+      <c r="I19">
         <v>17</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>28</v>
       </c>
       <c r="B20">
+        <v>12471</v>
+      </c>
+      <c r="C20">
         <v>217</v>
       </c>
-      <c r="C20">
+      <c r="D20">
         <v>4316</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>2722</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>89</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>191</v>
       </c>
-      <c r="G20">
+      <c r="H20">
         <v>87</v>
       </c>
-      <c r="H20">
+      <c r="I20">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>28</v>
       </c>
       <c r="B21">
+        <v>12689</v>
+      </c>
+      <c r="C21">
         <v>229</v>
       </c>
-      <c r="C21">
+      <c r="D21">
         <v>4540</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>3046</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>99</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>202</v>
       </c>
-      <c r="G21">
+      <c r="H21">
         <v>104</v>
       </c>
-      <c r="H21">
+      <c r="I21">
         <v>17</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>28</v>
       </c>
       <c r="B22">
+        <v>12858</v>
+      </c>
+      <c r="C22">
         <v>240</v>
       </c>
-      <c r="C22">
+      <c r="D22">
         <v>4622</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>2978</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>89</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>211</v>
       </c>
-      <c r="G22">
+      <c r="H22">
         <v>86</v>
       </c>
-      <c r="H22">
+      <c r="I22">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>28</v>
       </c>
       <c r="B23">
+        <v>13180</v>
+      </c>
+      <c r="C23">
         <v>253</v>
       </c>
-      <c r="C23">
+      <c r="D23">
         <v>4807</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>3341</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>99</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>221</v>
       </c>
-      <c r="G23">
+      <c r="H23">
         <v>104</v>
       </c>
-      <c r="H23">
+      <c r="I23">
         <v>17</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>28</v>
       </c>
       <c r="B24">
+        <v>13497</v>
+      </c>
+      <c r="C24">
         <v>265</v>
       </c>
-      <c r="C24">
+      <c r="D24">
         <v>5054</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>3532</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>99</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>231</v>
       </c>
-      <c r="G24">
+      <c r="H24">
         <v>103</v>
       </c>
-      <c r="H24">
+      <c r="I24">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>28</v>
       </c>
       <c r="B25">
+        <v>13885</v>
+      </c>
+      <c r="C25">
         <v>277</v>
       </c>
-      <c r="C25">
+      <c r="D25">
         <v>5347</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>3742</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>108</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>241</v>
       </c>
-      <c r="G25">
+      <c r="H25">
         <v>116</v>
       </c>
-      <c r="H25">
+      <c r="I25">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>28</v>
       </c>
       <c r="B26">
+        <v>14152</v>
+      </c>
+      <c r="C26">
         <v>288</v>
       </c>
-      <c r="C26">
+      <c r="D26">
         <v>5586</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>3062</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>90</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>250</v>
       </c>
-      <c r="G26">
+      <c r="H26">
         <v>93</v>
       </c>
-      <c r="H26">
+      <c r="I26">
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>28</v>
       </c>
       <c r="B27">
+        <v>14399</v>
+      </c>
+      <c r="C27">
         <v>302</v>
       </c>
-      <c r="C27">
+      <c r="D27">
         <v>5789</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>3338</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>100</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>260</v>
       </c>
-      <c r="G27">
+      <c r="H27">
         <v>106</v>
       </c>
-      <c r="H27">
+      <c r="I27">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>28</v>
       </c>
       <c r="B28">
+        <v>14585</v>
+      </c>
+      <c r="C28">
         <v>315</v>
       </c>
-      <c r="C28">
+      <c r="D28">
         <v>6140</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>3407</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>99</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>270</v>
       </c>
-      <c r="G28">
+      <c r="H28">
         <v>106</v>
       </c>
-      <c r="H28">
+      <c r="I28">
         <v>17</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
       <c r="B29">
+        <v>14873</v>
+      </c>
+      <c r="C29">
         <v>325</v>
       </c>
-      <c r="C29">
+      <c r="D29">
         <v>6351</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>3768</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>109</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>280</v>
       </c>
-      <c r="G29">
+      <c r="H29">
         <v>118</v>
       </c>
-      <c r="H29">
+      <c r="I29">
         <v>17</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
       <c r="B30">
+        <v>15192</v>
+      </c>
+      <c r="C30">
         <v>337</v>
       </c>
-      <c r="C30">
+      <c r="D30">
         <v>6639</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>3539</v>
       </c>
-      <c r="E30">
+      <c r="F30">
         <v>99</v>
       </c>
-      <c r="F30">
+      <c r="G30">
         <v>290</v>
       </c>
-      <c r="G30">
+      <c r="H30">
         <v>110</v>
       </c>
-      <c r="H30">
+      <c r="I30">
         <v>17</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
       <c r="B31">
+        <v>15611</v>
+      </c>
+      <c r="C31">
         <v>350</v>
       </c>
-      <c r="C31">
+      <c r="D31">
         <v>6896</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>3769</v>
       </c>
-      <c r="E31">
+      <c r="F31">
         <v>109</v>
       </c>
-      <c r="F31">
+      <c r="G31">
         <v>299</v>
       </c>
-      <c r="G31">
+      <c r="H31">
         <v>121</v>
       </c>
-      <c r="H31">
+      <c r="I31">
         <v>17</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>28</v>
       </c>
       <c r="B32">
+        <v>15626</v>
+      </c>
+      <c r="C32">
         <v>360</v>
       </c>
-      <c r="C32">
+      <c r="D32">
         <v>6959</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>4105</v>
       </c>
-      <c r="E32">
+      <c r="F32">
         <v>110</v>
       </c>
-      <c r="F32">
+      <c r="G32">
         <v>309</v>
       </c>
-      <c r="G32">
+      <c r="H32">
         <v>123</v>
       </c>
-      <c r="H32">
+      <c r="I32">
         <v>17</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>28</v>
       </c>
       <c r="B33">
+        <v>15970</v>
+      </c>
+      <c r="C33">
         <v>374</v>
       </c>
-      <c r="C33">
+      <c r="D33">
         <v>7183</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>4404</v>
       </c>
-      <c r="E33">
+      <c r="F33">
         <v>119</v>
       </c>
-      <c r="F33">
+      <c r="G33">
         <v>319</v>
       </c>
-      <c r="G33">
+      <c r="H33">
         <v>131</v>
       </c>
-      <c r="H33">
+      <c r="I33">
         <v>17</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>28</v>
       </c>
       <c r="B34">
+        <v>16303</v>
+      </c>
+      <c r="C34">
         <v>388</v>
       </c>
-      <c r="C34">
+      <c r="D34">
         <v>7382</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>3173</v>
       </c>
-      <c r="E34">
+      <c r="F34">
         <v>91</v>
       </c>
-      <c r="F34">
+      <c r="G34">
         <v>328</v>
       </c>
-      <c r="G34">
+      <c r="H34">
         <v>100</v>
       </c>
-      <c r="H34">
+      <c r="I34">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>28</v>
       </c>
       <c r="B35">
+        <v>16685</v>
+      </c>
+      <c r="C35">
         <v>398</v>
       </c>
-      <c r="C35">
+      <c r="D35">
         <v>7698</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>3495</v>
       </c>
-      <c r="E35">
+      <c r="F35">
         <v>101</v>
       </c>
-      <c r="F35">
+      <c r="G35">
         <v>338</v>
       </c>
-      <c r="G35">
+      <c r="H35">
         <v>107</v>
       </c>
-      <c r="H35">
+      <c r="I35">
         <v>17</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>28</v>
       </c>
       <c r="B36">
+        <v>17062</v>
+      </c>
+      <c r="C36">
         <v>418</v>
       </c>
-      <c r="C36">
+      <c r="D36">
         <v>7942</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>3561</v>
       </c>
-      <c r="E36">
+      <c r="F36">
         <v>101</v>
       </c>
-      <c r="F36">
+      <c r="G36">
         <v>348</v>
       </c>
-      <c r="G36">
+      <c r="H36">
         <v>100</v>
       </c>
-      <c r="H36">
+      <c r="I36">
         <v>17</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>28</v>
       </c>
       <c r="B37">
+        <v>17153</v>
+      </c>
+      <c r="C37">
         <v>436</v>
       </c>
-      <c r="C37">
+      <c r="D37">
         <v>8148</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>3850</v>
       </c>
-      <c r="E37">
+      <c r="F37">
         <v>111</v>
       </c>
-      <c r="F37">
+      <c r="G37">
         <v>359</v>
       </c>
-      <c r="G37">
+      <c r="H37">
         <v>119</v>
       </c>
-      <c r="H37">
+      <c r="I37">
         <v>17</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>28</v>
       </c>
       <c r="B38">
+        <v>17582</v>
+      </c>
+      <c r="C38">
         <v>436</v>
       </c>
-      <c r="C38">
+      <c r="D38">
         <v>8304</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>3662</v>
       </c>
-      <c r="E38">
+      <c r="F38">
         <v>101</v>
       </c>
-      <c r="F38">
+      <c r="G38">
         <v>371</v>
       </c>
-      <c r="G38">
+      <c r="H38">
         <v>100</v>
       </c>
-      <c r="H38">
+      <c r="I38">
         <v>17</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>28</v>
       </c>
       <c r="B39">
+        <v>17856</v>
+      </c>
+      <c r="C39">
         <v>449</v>
       </c>
-      <c r="C39">
+      <c r="D39">
         <v>8595</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>3941</v>
       </c>
-      <c r="E39">
+      <c r="F39">
         <v>111</v>
       </c>
-      <c r="F39">
+      <c r="G39">
         <v>378</v>
       </c>
-      <c r="G39">
+      <c r="H39">
         <v>115</v>
       </c>
-      <c r="H39">
+      <c r="I39">
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>28</v>
       </c>
       <c r="B40">
+        <v>18087</v>
+      </c>
+      <c r="C40">
         <v>471</v>
       </c>
-      <c r="C40">
+      <c r="D40">
         <v>8816</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>4117</v>
       </c>
-      <c r="E40">
+      <c r="F40">
         <v>111</v>
       </c>
-      <c r="F40">
+      <c r="G40">
         <v>387</v>
       </c>
-      <c r="G40">
+      <c r="H40">
         <v>119</v>
       </c>
-      <c r="H40">
+      <c r="I40">
         <v>17</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>28</v>
       </c>
       <c r="B41">
+        <v>18394</v>
+      </c>
+      <c r="C41">
         <v>487</v>
       </c>
-      <c r="C41">
+      <c r="D41">
         <v>8995</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>4472</v>
       </c>
-      <c r="E41">
+      <c r="F41">
         <v>122</v>
       </c>
-      <c r="F41">
+      <c r="G41">
         <v>403</v>
       </c>
-      <c r="G41">
+      <c r="H41">
         <v>130</v>
       </c>
-      <c r="H41">
+      <c r="I41">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>28</v>
       </c>
       <c r="B42">
+        <v>18523</v>
+      </c>
+      <c r="C42">
         <v>500</v>
       </c>
-      <c r="C42">
+      <c r="D42">
         <v>9139</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>3928</v>
       </c>
-      <c r="E42">
+      <c r="F42">
         <v>102</v>
       </c>
-      <c r="G42">
+      <c r="H42">
         <v>102</v>
       </c>
-      <c r="H42">
+      <c r="I42">
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>28</v>
       </c>
       <c r="B43">
+        <v>18855</v>
+      </c>
+      <c r="C43">
         <v>503</v>
       </c>
-      <c r="C43">
+      <c r="D43">
         <v>9430</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>4297</v>
       </c>
-      <c r="E43">
+      <c r="F43">
         <v>112</v>
       </c>
-      <c r="G43">
+      <c r="H43">
         <v>118</v>
       </c>
-      <c r="H43">
+      <c r="I43">
         <v>17</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>28</v>
       </c>
       <c r="B44">
+        <v>19177</v>
+      </c>
+      <c r="C44">
         <v>514</v>
       </c>
-      <c r="C44">
+      <c r="D44">
         <v>9637</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>4400</v>
       </c>
-      <c r="E44">
+      <c r="F44">
         <v>112</v>
       </c>
-      <c r="G44">
+      <c r="H44">
         <v>121</v>
       </c>
-      <c r="H44">
+      <c r="I44">
         <v>17</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>28</v>
       </c>
       <c r="B45">
+        <v>19577</v>
+      </c>
+      <c r="C45">
         <v>537</v>
       </c>
-      <c r="C45">
+      <c r="D45">
         <v>10005</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>4671</v>
       </c>
-      <c r="E45">
+      <c r="F45">
         <v>125</v>
       </c>
-      <c r="G45">
+      <c r="H45">
         <v>128</v>
       </c>
-      <c r="H45">
+      <c r="I45">
         <v>17</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>28</v>
       </c>
       <c r="B46">
+        <v>19831</v>
+      </c>
+      <c r="C46">
         <v>533</v>
       </c>
-      <c r="C46">
+      <c r="D46">
         <v>10247</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>4517</v>
       </c>
-      <c r="E46">
+      <c r="F46">
         <v>113</v>
       </c>
-      <c r="G46">
+      <c r="H46">
         <v>120</v>
       </c>
-      <c r="H46">
+      <c r="I46">
         <v>17</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>28</v>
       </c>
       <c r="B47">
+        <v>20050</v>
+      </c>
+      <c r="C47">
         <v>546</v>
       </c>
-      <c r="C47">
+      <c r="D47">
         <v>10483</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>4835</v>
       </c>
-      <c r="E47">
+      <c r="F47">
         <v>122</v>
       </c>
-      <c r="G47">
+      <c r="H47">
         <v>134</v>
       </c>
-      <c r="H47">
+      <c r="I47">
         <v>17</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>28</v>
       </c>
       <c r="B48">
+        <v>20349</v>
+      </c>
+      <c r="C48">
         <v>559</v>
       </c>
-      <c r="C48">
+      <c r="D48">
         <v>10753</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>5000</v>
       </c>
-      <c r="E48">
+      <c r="F48">
         <v>125</v>
       </c>
-      <c r="G48">
+      <c r="H48">
         <v>128</v>
       </c>
-      <c r="H48">
+      <c r="I48">
         <v>17</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>28</v>
       </c>
       <c r="B49">
+        <v>20780</v>
+      </c>
+      <c r="C49">
         <v>589</v>
       </c>
-      <c r="C49">
+      <c r="D49">
         <v>10966</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>5307</v>
       </c>
-      <c r="E49">
+      <c r="F49">
         <v>139</v>
       </c>
-      <c r="G49">
+      <c r="H49">
         <v>139</v>
       </c>
-      <c r="H49">
+      <c r="I49">
         <v>17</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>28</v>
       </c>
       <c r="B50">
+        <v>21038</v>
+      </c>
+      <c r="C50">
         <v>583</v>
       </c>
-      <c r="C50">
+      <c r="D50">
         <v>11036</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>4010</v>
       </c>
-      <c r="E50">
+      <c r="F50">
         <v>103</v>
       </c>
-      <c r="G50">
+      <c r="H50">
         <v>112</v>
       </c>
-      <c r="H50">
+      <c r="I50">
         <v>17</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>28</v>
       </c>
       <c r="B51">
+        <v>21362</v>
+      </c>
+      <c r="C51">
         <v>594</v>
       </c>
-      <c r="C51">
+      <c r="D51">
         <v>11422</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>4346</v>
       </c>
-      <c r="E51">
+      <c r="F51">
         <v>114</v>
       </c>
-      <c r="G51">
+      <c r="H51">
         <v>119</v>
       </c>
-      <c r="H51">
+      <c r="I51">
         <v>17</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>28</v>
       </c>
       <c r="B52">
+        <v>21371</v>
+      </c>
+      <c r="C52">
         <v>623</v>
       </c>
-      <c r="C52">
+      <c r="D52">
         <v>11358</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>4361</v>
       </c>
-      <c r="E52">
+      <c r="F52">
         <v>93</v>
       </c>
-      <c r="G52">
+      <c r="H52">
         <v>94</v>
       </c>
-      <c r="H52">
+      <c r="I52">
         <v>17</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>28</v>
       </c>
       <c r="B53">
+        <v>21659</v>
+      </c>
+      <c r="C53">
         <v>618</v>
       </c>
-      <c r="C53">
+      <c r="D53">
         <v>11603</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>4580</v>
       </c>
-      <c r="E53">
+      <c r="F53">
         <v>103</v>
       </c>
-      <c r="G53">
+      <c r="H53">
         <v>107</v>
       </c>
-      <c r="H53">
+      <c r="I53">
         <v>17</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>28</v>
       </c>
       <c r="B54">
+        <v>21980</v>
+      </c>
+      <c r="C54">
         <v>646</v>
       </c>
-      <c r="C54">
+      <c r="D54">
         <v>11923</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>4474</v>
       </c>
-      <c r="E54">
+      <c r="F54">
         <v>93</v>
       </c>
-      <c r="G54">
+      <c r="H54">
         <v>94</v>
       </c>
-      <c r="H54">
+      <c r="I54">
         <v>17</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>28</v>
       </c>
       <c r="B55">
+        <v>22320</v>
+      </c>
+      <c r="C55">
         <v>644</v>
       </c>
-      <c r="C55">
+      <c r="D55">
         <v>12103</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>4812</v>
       </c>
-      <c r="E55">
+      <c r="F55">
         <v>103</v>
       </c>
-      <c r="G55">
+      <c r="H55">
         <v>110</v>
       </c>
-      <c r="H55">
+      <c r="I55">
         <v>17</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>28</v>
       </c>
       <c r="B56">
+        <v>22608</v>
+      </c>
+      <c r="C56">
         <v>657</v>
       </c>
-      <c r="C56">
+      <c r="D56">
         <v>12315</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>4808</v>
       </c>
-      <c r="E56">
+      <c r="F56">
         <v>103</v>
       </c>
-      <c r="G56">
+      <c r="H56">
         <v>106</v>
       </c>
-      <c r="H56">
+      <c r="I56">
         <v>17</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>28</v>
       </c>
       <c r="B57">
+        <v>22964</v>
+      </c>
+      <c r="C57">
         <v>671</v>
       </c>
-      <c r="C57">
+      <c r="D57">
         <v>12773</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>5046</v>
       </c>
-      <c r="E57">
+      <c r="F57">
         <v>113</v>
       </c>
-      <c r="G57">
+      <c r="H57">
         <v>121</v>
       </c>
-      <c r="H57">
+      <c r="I57">
         <v>17</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>28</v>
       </c>
       <c r="B58">
+        <v>23293</v>
+      </c>
+      <c r="C58">
         <v>690</v>
       </c>
-      <c r="C58">
+      <c r="D58">
         <v>13024</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>4426</v>
       </c>
-      <c r="E58">
+      <c r="F58">
         <v>94</v>
       </c>
-      <c r="G58">
+      <c r="H58">
         <v>97</v>
       </c>
-      <c r="H58">
+      <c r="I58">
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>28</v>
       </c>
       <c r="B59">
+        <v>23428</v>
+      </c>
+      <c r="C59">
         <v>691</v>
       </c>
-      <c r="C59">
+      <c r="D59">
         <v>12945</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>4757</v>
       </c>
-      <c r="E59">
+      <c r="F59">
         <v>104</v>
       </c>
-      <c r="G59">
+      <c r="H59">
         <v>112</v>
       </c>
-      <c r="H59">
+      <c r="I59">
         <v>17</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>28</v>
       </c>
       <c r="B60">
+        <v>23832</v>
+      </c>
+      <c r="C60">
         <v>726</v>
       </c>
-      <c r="C60">
+      <c r="D60">
         <v>13485</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>4869</v>
       </c>
-      <c r="E60">
+      <c r="F60">
         <v>104</v>
       </c>
-      <c r="G60">
+      <c r="H60">
         <v>108</v>
       </c>
-      <c r="H60">
+      <c r="I60">
         <v>17</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>28</v>
       </c>
       <c r="B61">
+        <v>24016</v>
+      </c>
+      <c r="C61">
         <v>725</v>
       </c>
-      <c r="C61">
+      <c r="D61">
         <v>13891</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>5154</v>
       </c>
-      <c r="E61">
+      <c r="F61">
         <v>114</v>
       </c>
-      <c r="G61">
+      <c r="H61">
         <v>119</v>
       </c>
-      <c r="H61">
+      <c r="I61">
         <v>17</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>28</v>
       </c>
       <c r="B62">
+        <v>24142</v>
+      </c>
+      <c r="C62">
         <v>742</v>
       </c>
-      <c r="C62">
+      <c r="D62">
         <v>14363</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>5094</v>
       </c>
-      <c r="E62">
+      <c r="F62">
         <v>104</v>
       </c>
-      <c r="G62">
+      <c r="H62">
         <v>106</v>
       </c>
-      <c r="H62">
+      <c r="I62">
         <v>17</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>28</v>
       </c>
       <c r="B63">
+        <v>24540</v>
+      </c>
+      <c r="C63">
         <v>738</v>
       </c>
-      <c r="C63">
+      <c r="D63">
         <v>13968</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>5350</v>
       </c>
-      <c r="E63">
+      <c r="F63">
         <v>116</v>
       </c>
-      <c r="G63">
+      <c r="H63">
         <v>119</v>
       </c>
-      <c r="H63">
+      <c r="I63">
         <v>17</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>28</v>
       </c>
       <c r="B64">
+        <v>24940</v>
+      </c>
+      <c r="C64">
         <v>764</v>
       </c>
-      <c r="C64">
+      <c r="D64">
         <v>14345</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>5597</v>
       </c>
-      <c r="E64">
+      <c r="F64">
         <v>115</v>
       </c>
-      <c r="G64">
+      <c r="H64">
         <v>117</v>
       </c>
-      <c r="H64">
+      <c r="I64">
         <v>17</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>28</v>
       </c>
       <c r="B65">
+        <v>25173</v>
+      </c>
+      <c r="C65">
         <v>761</v>
       </c>
-      <c r="C65">
+      <c r="D65">
         <v>15087</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>5921</v>
       </c>
-      <c r="E65">
+      <c r="F65">
         <v>126</v>
       </c>
-      <c r="G65">
+      <c r="H65">
         <v>138</v>
       </c>
-      <c r="H65">
+      <c r="I65">
         <v>17</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>28</v>
       </c>
       <c r="B66">
+        <v>25622</v>
+      </c>
+      <c r="C66">
         <v>785</v>
       </c>
-      <c r="C66">
+      <c r="D66">
         <v>14872</v>
       </c>
-      <c r="D66">
+      <c r="E66">
         <v>3856</v>
       </c>
-      <c r="E66">
+      <c r="F66">
         <v>85</v>
       </c>
-      <c r="G66">
+      <c r="H66">
         <v>73</v>
       </c>
-      <c r="H66">
+      <c r="I66">
         <v>17</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>28</v>
       </c>
       <c r="B67">
+        <v>25980</v>
+      </c>
+      <c r="C67">
         <v>785</v>
       </c>
-      <c r="C67">
+      <c r="D67">
         <v>15057</v>
       </c>
-      <c r="D67">
+      <c r="E67">
         <v>4173</v>
       </c>
-      <c r="E67">
+      <c r="F67">
         <v>95</v>
       </c>
-      <c r="G67">
+      <c r="H67">
         <v>101</v>
       </c>
-      <c r="H67">
+      <c r="I67">
         <v>17</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>28</v>
       </c>
       <c r="B68">
+        <v>26073</v>
+      </c>
+      <c r="C68">
         <v>813</v>
       </c>
-      <c r="C68">
+      <c r="D68">
         <v>15287</v>
       </c>
-      <c r="D68">
+      <c r="E68">
         <v>4362</v>
       </c>
-      <c r="E68">
+      <c r="F68">
         <v>95</v>
       </c>
-      <c r="G68">
+      <c r="H68">
         <v>95</v>
       </c>
-      <c r="H68">
+      <c r="I68">
         <v>17</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>28</v>
       </c>
       <c r="B69">
+        <v>26384</v>
+      </c>
+      <c r="C69">
         <v>819</v>
       </c>
-      <c r="C69">
+      <c r="D69">
         <v>15505</v>
       </c>
-      <c r="D69">
+      <c r="E69">
         <v>4653</v>
       </c>
-      <c r="E69">
+      <c r="F69">
         <v>105</v>
       </c>
-      <c r="G69">
+      <c r="H69">
         <v>110</v>
       </c>
-      <c r="H69">
+      <c r="I69">
         <v>17</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>28</v>
       </c>
       <c r="B70">
+        <v>26782</v>
+      </c>
+      <c r="C70">
         <v>845</v>
       </c>
-      <c r="C70">
+      <c r="D70">
         <v>15618</v>
       </c>
-      <c r="D70">
+      <c r="E70">
         <v>4422</v>
       </c>
-      <c r="E70">
+      <c r="F70">
         <v>95</v>
       </c>
-      <c r="G70">
+      <c r="H70">
         <v>84</v>
       </c>
-      <c r="H70">
+      <c r="I70">
         <v>17</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>28</v>
       </c>
       <c r="B71">
+        <v>27032</v>
+      </c>
+      <c r="C71">
         <v>834</v>
       </c>
-      <c r="C71">
+      <c r="D71">
         <v>16027</v>
       </c>
-      <c r="D71">
+      <c r="E71">
         <v>4734</v>
       </c>
-      <c r="E71">
+      <c r="F71">
         <v>105</v>
       </c>
-      <c r="G71">
+      <c r="H71">
         <v>104</v>
       </c>
-      <c r="H71">
+      <c r="I71">
         <v>17</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>28</v>
       </c>
       <c r="B72">
+        <v>27206</v>
+      </c>
+      <c r="C72">
         <v>868</v>
       </c>
-      <c r="C72">
+      <c r="D72">
         <v>16087</v>
       </c>
-      <c r="D72">
+      <c r="E72">
         <v>4894</v>
       </c>
-      <c r="E72">
+      <c r="F72">
         <v>105</v>
       </c>
-      <c r="G72">
+      <c r="H72">
         <v>107</v>
       </c>
-      <c r="H72">
+      <c r="I72">
         <v>17</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>28</v>
       </c>
       <c r="B73">
+        <v>27449</v>
+      </c>
+      <c r="C73">
         <v>859</v>
       </c>
-      <c r="C73">
+      <c r="D73">
         <v>16261</v>
       </c>
-      <c r="D73">
+      <c r="E73">
         <v>5183</v>
       </c>
-      <c r="E73">
+      <c r="F73">
         <v>115</v>
       </c>
-      <c r="G73">
+      <c r="H73">
         <v>119</v>
       </c>
-      <c r="H73">
+      <c r="I73">
         <v>17</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>28</v>
       </c>
       <c r="B74">
+        <v>27852</v>
+      </c>
+      <c r="C74">
         <v>971</v>
       </c>
-      <c r="C74">
+      <c r="D74">
         <v>16452</v>
       </c>
-      <c r="D74">
+      <c r="E74">
         <v>4568</v>
       </c>
-      <c r="E74">
+      <c r="F74">
         <v>96</v>
       </c>
-      <c r="G74">
+      <c r="H74">
         <v>79</v>
       </c>
-      <c r="H74">
+      <c r="I74">
         <v>17</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>28</v>
       </c>
       <c r="B75">
+        <v>28114</v>
+      </c>
+      <c r="C75">
         <v>943</v>
       </c>
-      <c r="C75">
+      <c r="D75">
         <v>16658</v>
       </c>
-      <c r="D75">
+      <c r="E75">
         <v>4866</v>
       </c>
-      <c r="E75">
+      <c r="F75">
         <v>106</v>
       </c>
-      <c r="G75">
+      <c r="H75">
         <v>103</v>
       </c>
-      <c r="H75">
+      <c r="I75">
         <v>17</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>28</v>
       </c>
       <c r="B76">
+        <v>28349</v>
+      </c>
+      <c r="C76">
         <v>1074</v>
       </c>
-      <c r="C76">
+      <c r="D76">
         <v>17113</v>
       </c>
-      <c r="D76">
+      <c r="E76">
         <v>4919</v>
       </c>
-      <c r="E76">
+      <c r="F76">
         <v>106</v>
       </c>
-      <c r="G76">
+      <c r="H76">
         <v>105</v>
       </c>
-      <c r="H76">
+      <c r="I76">
         <v>17</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>28</v>
       </c>
       <c r="B77">
+        <v>28693</v>
+      </c>
+      <c r="C77">
         <v>1062</v>
       </c>
-      <c r="C77">
+      <c r="D77">
         <v>17208</v>
       </c>
-      <c r="D77">
+      <c r="E77">
         <v>5186</v>
       </c>
-      <c r="E77">
+      <c r="F77">
         <v>121</v>
       </c>
-      <c r="G77">
+      <c r="H77">
         <v>114</v>
       </c>
-      <c r="H77">
+      <c r="I77">
         <v>17</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>28</v>
       </c>
       <c r="B78">
+        <v>29092</v>
+      </c>
+      <c r="C78">
         <v>1096</v>
       </c>
-      <c r="C78">
+      <c r="D78">
         <v>17319</v>
       </c>
-      <c r="D78">
+      <c r="E78">
         <v>5057</v>
       </c>
-      <c r="E78">
+      <c r="F78">
         <v>110</v>
       </c>
-      <c r="G78">
+      <c r="H78">
         <v>104</v>
       </c>
-      <c r="H78">
+      <c r="I78">
         <v>17</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>28</v>
       </c>
       <c r="B79">
+        <v>29304</v>
+      </c>
+      <c r="C79">
         <v>1053</v>
       </c>
-      <c r="C79">
+      <c r="D79">
         <v>17733</v>
       </c>
-      <c r="D79">
+      <c r="E79">
         <v>5369</v>
       </c>
-      <c r="E79">
+      <c r="F79">
         <v>120</v>
       </c>
-      <c r="G79">
+      <c r="H79">
         <v>117</v>
       </c>
-      <c r="H79">
+      <c r="I79">
         <v>17</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>28</v>
       </c>
       <c r="B80">
+        <v>29582</v>
+      </c>
+      <c r="C80">
         <v>1061</v>
       </c>
-      <c r="C80">
+      <c r="D80">
         <v>18072</v>
       </c>
-      <c r="D80">
+      <c r="E80">
         <v>5632</v>
       </c>
-      <c r="E80">
+      <c r="F80">
         <v>121</v>
       </c>
-      <c r="G80">
+      <c r="H80">
         <v>119</v>
       </c>
-      <c r="H80">
+      <c r="I80">
         <v>17</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>28</v>
       </c>
       <c r="B81">
+        <v>29752</v>
+      </c>
+      <c r="C81">
         <v>1101</v>
       </c>
-      <c r="C81">
+      <c r="D81">
         <v>18269</v>
       </c>
-      <c r="D81">
+      <c r="E81">
         <v>6394</v>
       </c>
-      <c r="E81">
+      <c r="F81">
         <v>136</v>
       </c>
-      <c r="G81">
+      <c r="H81">
         <v>130</v>
       </c>
-      <c r="H81">
+      <c r="I81">
         <v>17</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>28</v>
       </c>
       <c r="B82">
+        <v>29995</v>
+      </c>
+      <c r="C82">
         <v>1106</v>
       </c>
-      <c r="C82">
+      <c r="D82">
         <v>18417</v>
       </c>
-      <c r="D82">
+      <c r="E82">
         <v>4880</v>
       </c>
-      <c r="E82">
+      <c r="F82">
         <v>100</v>
       </c>
-      <c r="G82">
+      <c r="H82">
         <v>73</v>
       </c>
-      <c r="H82">
+      <c r="I82">
         <v>17</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>28</v>
       </c>
       <c r="B83">
+        <v>30314</v>
+      </c>
+      <c r="C83">
         <v>1129</v>
       </c>
-      <c r="C83">
+      <c r="D83">
         <v>18473</v>
       </c>
-      <c r="D83">
+      <c r="E83">
         <v>5109</v>
       </c>
-      <c r="E83">
+      <c r="F83">
         <v>110</v>
       </c>
-      <c r="G83">
+      <c r="H83">
         <v>101</v>
       </c>
-      <c r="H83">
+      <c r="I83">
         <v>17</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>28</v>
       </c>
       <c r="B84">
+        <v>30737</v>
+      </c>
+      <c r="C84">
         <v>1139</v>
       </c>
-      <c r="C84">
+      <c r="D84">
         <v>18575</v>
       </c>
-      <c r="D84">
+      <c r="E84">
         <v>5187</v>
       </c>
-      <c r="E84">
+      <c r="F84">
         <v>110</v>
       </c>
-      <c r="G84">
+      <c r="H84">
         <v>105</v>
       </c>
-      <c r="H84">
+      <c r="I84">
         <v>17</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>28</v>
       </c>
       <c r="B85">
+        <v>31031</v>
+      </c>
+      <c r="C85">
         <v>1112</v>
       </c>
-      <c r="C85">
+      <c r="D85">
         <v>19232</v>
       </c>
-      <c r="D85">
+      <c r="E85">
         <v>5464</v>
       </c>
-      <c r="E85">
+      <c r="F85">
         <v>121</v>
       </c>
-      <c r="G85">
+      <c r="H85">
         <v>116</v>
       </c>
-      <c r="H85">
+      <c r="I85">
         <v>17</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>28</v>
       </c>
       <c r="B86">
+        <v>31380</v>
+      </c>
+      <c r="C86">
         <v>1225</v>
       </c>
-      <c r="C86">
+      <c r="D86">
         <v>19420</v>
       </c>
-      <c r="D86">
+      <c r="E86">
         <v>5339</v>
       </c>
-      <c r="E86">
+      <c r="F86">
         <v>110</v>
       </c>
-      <c r="G86">
+      <c r="H86">
         <v>103</v>
       </c>
-      <c r="H86">
+      <c r="I86">
         <v>17</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>28</v>
       </c>
       <c r="B87">
+        <v>31709</v>
+      </c>
+      <c r="C87">
         <v>1193</v>
       </c>
-      <c r="C87">
+      <c r="D87">
         <v>19689</v>
       </c>
-      <c r="D87">
+      <c r="E87">
         <v>5593</v>
       </c>
-      <c r="E87">
+      <c r="F87">
         <v>121</v>
       </c>
-      <c r="G87">
+      <c r="H87">
         <v>118</v>
       </c>
-      <c r="H87">
+      <c r="I87">
         <v>17</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>28</v>
       </c>
       <c r="B88">
+        <v>31798</v>
+      </c>
+      <c r="C88">
         <v>1197</v>
       </c>
-      <c r="C88">
+      <c r="D88">
         <v>19883</v>
       </c>
-      <c r="D88">
+      <c r="E88">
         <v>5786</v>
       </c>
-      <c r="E88">
+      <c r="F88">
         <v>121</v>
       </c>
-      <c r="G88">
+      <c r="H88">
         <v>117</v>
       </c>
-      <c r="H88">
+      <c r="I88">
         <v>17</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>28</v>
       </c>
       <c r="B89">
+        <v>32357</v>
+      </c>
+      <c r="C89">
         <v>1243</v>
       </c>
-      <c r="C89">
+      <c r="D89">
         <v>20094</v>
       </c>
-      <c r="D89">
+      <c r="E89">
         <v>6078</v>
       </c>
-      <c r="E89">
+      <c r="F89">
         <v>131</v>
       </c>
-      <c r="G89">
+      <c r="H89">
         <v>132</v>
       </c>
-      <c r="H89">
+      <c r="I89">
         <v>17</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>28</v>
       </c>
       <c r="B90">
+        <v>32450</v>
+      </c>
+      <c r="C90">
         <v>1370</v>
       </c>
-      <c r="C90">
+      <c r="D90">
         <v>20261</v>
       </c>
-      <c r="D90">
+      <c r="E90">
         <v>5506</v>
       </c>
-      <c r="E90">
+      <c r="F90">
         <v>113</v>
       </c>
-      <c r="G90">
+      <c r="H90">
         <v>108</v>
       </c>
-      <c r="H90">
+      <c r="I90">
         <v>17</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>28</v>
       </c>
       <c r="B91">
+        <v>32773</v>
+      </c>
+      <c r="C91">
         <v>1368</v>
       </c>
-      <c r="C91">
+      <c r="D91">
         <v>20531</v>
       </c>
-      <c r="D91">
+      <c r="E91">
         <v>5778</v>
       </c>
-      <c r="E91">
+      <c r="F91">
         <v>120</v>
       </c>
-      <c r="G91">
+      <c r="H91">
         <v>120</v>
       </c>
-      <c r="H91">
+      <c r="I91">
         <v>17</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>28</v>
       </c>
       <c r="B92">
+        <v>32881</v>
+      </c>
+      <c r="C92">
         <v>1392</v>
       </c>
-      <c r="C92">
+      <c r="D92">
         <v>20622</v>
       </c>
-      <c r="D92">
+      <c r="E92">
         <v>5888</v>
       </c>
-      <c r="E92">
+      <c r="F92">
         <v>121</v>
       </c>
-      <c r="G92">
+      <c r="H92">
         <v>121</v>
       </c>
-      <c r="H92">
+      <c r="I92">
         <v>17</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>28</v>
       </c>
       <c r="B93">
+        <v>33199</v>
+      </c>
+      <c r="C93">
         <v>1411</v>
       </c>
-      <c r="C93">
+      <c r="D93">
         <v>20838</v>
       </c>
-      <c r="D93">
+      <c r="E93">
         <v>6153</v>
       </c>
-      <c r="E93">
+      <c r="F93">
         <v>130</v>
       </c>
-      <c r="G93">
+      <c r="H93">
         <v>140</v>
       </c>
-      <c r="H93">
+      <c r="I93">
         <v>17</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>28</v>
       </c>
       <c r="B94">
+        <v>33573</v>
+      </c>
+      <c r="C94">
         <v>1451</v>
       </c>
-      <c r="C94">
+      <c r="D94">
         <v>20890</v>
       </c>
-      <c r="D94">
+      <c r="E94">
         <v>5974</v>
       </c>
-      <c r="E94">
+      <c r="F94">
         <v>120</v>
       </c>
-      <c r="G94">
+      <c r="H94">
         <v>115</v>
       </c>
-      <c r="H94">
+      <c r="I94">
         <v>17</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>28</v>
       </c>
       <c r="B95">
+        <v>33869</v>
+      </c>
+      <c r="C95">
         <v>1389</v>
       </c>
-      <c r="C95">
+      <c r="D95">
         <v>21338</v>
       </c>
-      <c r="D95">
+      <c r="E95">
         <v>6277</v>
       </c>
-      <c r="E95">
+      <c r="F95">
         <v>130</v>
       </c>
-      <c r="G95">
+      <c r="H95">
         <v>138</v>
       </c>
-      <c r="H95">
+      <c r="I95">
         <v>17</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>28</v>
       </c>
       <c r="B96">
+        <v>34261</v>
+      </c>
+      <c r="C96">
         <v>1436</v>
       </c>
-      <c r="C96">
+      <c r="D96">
         <v>21711</v>
       </c>
-      <c r="D96">
+      <c r="E96">
         <v>6503</v>
       </c>
-      <c r="E96">
+      <c r="F96">
         <v>132</v>
       </c>
-      <c r="G96">
+      <c r="H96">
         <v>127</v>
       </c>
-      <c r="H96">
+      <c r="I96">
         <v>17</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>28</v>
       </c>
       <c r="B97">
+        <v>34517</v>
+      </c>
+      <c r="C97">
         <v>1449</v>
       </c>
-      <c r="C97">
+      <c r="D97">
         <v>21958</v>
       </c>
-      <c r="D97">
+      <c r="E97">
         <v>6927</v>
       </c>
-      <c r="E97">
+      <c r="F97">
         <v>146</v>
       </c>
-      <c r="G97">
+      <c r="H97">
         <v>144</v>
       </c>
-      <c r="H97">
+      <c r="I97">
         <v>17</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>28</v>
       </c>
       <c r="B98">
+        <v>34807</v>
+      </c>
+      <c r="C98">
         <v>1498</v>
       </c>
-      <c r="C98">
+      <c r="D98">
         <v>22072</v>
       </c>
-      <c r="D98">
+      <c r="E98">
         <v>4830</v>
       </c>
-      <c r="E98">
+      <c r="F98">
         <v>99</v>
       </c>
-      <c r="G98">
+      <c r="H98">
         <v>94</v>
       </c>
-      <c r="H98">
+      <c r="I98">
         <v>17</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>28</v>
       </c>
       <c r="B99">
+        <v>34997</v>
+      </c>
+      <c r="C99">
         <v>1500</v>
       </c>
-      <c r="C99">
+      <c r="D99">
         <v>22400</v>
       </c>
-      <c r="D99">
+      <c r="E99">
         <v>5126</v>
       </c>
-      <c r="E99">
+      <c r="F99">
         <v>109</v>
       </c>
-      <c r="G99">
+      <c r="H99">
         <v>114</v>
       </c>
-      <c r="H99">
+      <c r="I99">
         <v>17</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>28</v>
       </c>
       <c r="B100">
+        <v>35332</v>
+      </c>
+      <c r="C100">
         <v>1494</v>
       </c>
-      <c r="C100">
+      <c r="D100">
         <v>22555</v>
       </c>
-      <c r="D100">
+      <c r="E100">
         <v>5275</v>
       </c>
-      <c r="E100">
+      <c r="F100">
         <v>110</v>
       </c>
-      <c r="G100">
+      <c r="H100">
         <v>111</v>
       </c>
-      <c r="H100">
+      <c r="I100">
         <v>17</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>28</v>
       </c>
       <c r="B101">
+        <v>35714</v>
+      </c>
+      <c r="C101">
         <v>1464</v>
       </c>
-      <c r="C101">
+      <c r="D101">
         <v>22760</v>
       </c>
-      <c r="D101">
+      <c r="E101">
         <v>5553</v>
       </c>
-      <c r="E101">
+      <c r="F101">
         <v>119</v>
       </c>
-      <c r="G101">
+      <c r="H101">
         <v>121</v>
       </c>
-      <c r="H101">
+      <c r="I101">
         <v>17</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="E102" t="s">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
         <v>10</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>10</v>
       </c>
     </row>

</xml_diff>